<commit_message>
commit data, update xlsx, create digital res in nb
</commit_message>
<xml_diff>
--- a/dave-simple2.xlsx
+++ b/dave-simple2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
   <si>
     <t xml:space="preserve">Our Result</t>
   </si>
@@ -345,6 +345,19 @@
   </si>
   <si>
     <t xml:space="preserve">GANJ-5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{'PIET-1': {'P&gt;|t|': ' 0.001', 't': '    3.442', 'rsquared_adj': '0.104', 'nobs': '461'}, 'MAC-1': {'P&gt;|t|': ' 0.001', 't': '    3.217', 'rsquared_adj': '0.0822', 'nobs': '428'}, 'MAC-2': {'P&gt;|t|': ' 0.001', 't': '    3.341', 'rsquared_adj': '0.0918', 'nobs': '336'}, 'MAC-3': {'P&gt;|t|': ' 0.218', 't': '    1.243', 'rsquared_adj': '0.08', 'nobs': ' 92'}, 'GANJ-1': {'P&gt;|t|': ' 0.257', 't': '   -1.134', 'rsquared_adj': '0.0918', 'nobs': '428'}, 'GANJ-2': {'P&gt;|t|': ' 0.156', 't': '   -1.425', 'rsquared_adj': '0.0854', 'nobs': '188'}, 'GANJ-3': {'P&gt;|t|': ' 0.972', 't': '   -0.035', 'rsquared_adj': '0.0883', 'nobs': '355'}, 'GANJ-4': {'P&gt;|t|': ' 0.467', 't': '   -0.730', 'rsquared_adj': '0.097', 'nobs': '145'}, 'GANJ-5': {'P&gt;|t|': ' 0.520', 't': '   -0.650', 'rsquared_adj': '-0.102', 'nobs': ' 43'}}
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Our Result (FS )</t>
@@ -435,10 +448,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
@@ -530,7 +544,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -595,8 +609,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -708,10 +726,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1771,8 +1789,12 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="38.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C24" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="25" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2799,21 +2821,21 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="M1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
       <c r="R1" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -2845,7 +2867,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
@@ -2856,11 +2878,11 @@
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>8</v>
@@ -2871,11 +2893,11 @@
       <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>8</v>
@@ -2920,30 +2942,30 @@
         <v>0.073</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="18" t="n">
+        <v>53</v>
+      </c>
+      <c r="J3" s="19" t="n">
         <v>515</v>
       </c>
-      <c r="K3" s="18" t="n">
+      <c r="K3" s="19" t="n">
         <v>3.674</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="20" t="n">
+      <c r="M3" s="21" t="n">
         <v>0.092</v>
       </c>
-      <c r="N3" s="20" t="n">
+      <c r="N3" s="21" t="n">
         <v>0.001</v>
       </c>
-      <c r="O3" s="20" t="n">
+      <c r="O3" s="21" t="n">
         <v>458</v>
       </c>
-      <c r="P3" s="20" t="n">
+      <c r="P3" s="21" t="n">
         <v>3.478</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="10"/>
@@ -2985,40 +3007,40 @@
       <c r="J4" s="12" t="n">
         <v>409</v>
       </c>
-      <c r="K4" s="18" t="n">
+      <c r="K4" s="19" t="n">
         <v>2.913</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="22" t="n">
+      <c r="M4" s="23" t="n">
         <v>0.095</v>
       </c>
-      <c r="N4" s="22" t="n">
+      <c r="N4" s="23" t="n">
         <v>0.003</v>
       </c>
-      <c r="O4" s="22" t="n">
+      <c r="O4" s="23" t="n">
         <v>407</v>
       </c>
-      <c r="P4" s="22" t="n">
+      <c r="P4" s="23" t="n">
         <v>3.019</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="22" t="n">
+      <c r="R4" s="23" t="n">
         <v>0.106</v>
       </c>
-      <c r="S4" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="T4" s="22" t="n">
+      <c r="S4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="23" t="n">
         <v>457</v>
       </c>
-      <c r="U4" s="22" t="n">
+      <c r="U4" s="23" t="n">
         <v>4.246</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="W4" s="1"/>
@@ -3052,43 +3074,43 @@
       <c r="I5" s="8" t="n">
         <v>0.002</v>
       </c>
-      <c r="J5" s="18" t="n">
+      <c r="J5" s="19" t="n">
         <v>321</v>
       </c>
-      <c r="K5" s="18" t="n">
+      <c r="K5" s="19" t="n">
         <v>3.152</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="22" t="n">
+      <c r="M5" s="23" t="n">
         <v>0.121</v>
       </c>
-      <c r="N5" s="22" t="n">
+      <c r="N5" s="23" t="n">
         <v>0.001</v>
       </c>
-      <c r="O5" s="22" t="n">
+      <c r="O5" s="23" t="n">
         <v>326</v>
       </c>
-      <c r="P5" s="22" t="n">
+      <c r="P5" s="23" t="n">
         <v>3.44</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="22" t="n">
+      <c r="R5" s="23" t="n">
         <v>0.124</v>
       </c>
-      <c r="S5" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="22" t="n">
+      <c r="S5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="23" t="n">
         <v>363</v>
       </c>
-      <c r="U5" s="22" t="n">
+      <c r="U5" s="23" t="n">
         <v>4.217</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="V5" s="22" t="s">
         <v>20</v>
       </c>
       <c r="W5" s="1"/>
@@ -3122,43 +3144,43 @@
       <c r="I6" s="8" t="n">
         <v>0.608</v>
       </c>
-      <c r="J6" s="18" t="n">
+      <c r="J6" s="19" t="n">
         <v>88</v>
       </c>
-      <c r="K6" s="18" t="n">
+      <c r="K6" s="19" t="n">
         <v>0.516</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="22" t="n">
+      <c r="M6" s="23" t="n">
         <v>-0.023</v>
       </c>
-      <c r="N6" s="22" t="n">
+      <c r="N6" s="23" t="n">
         <v>0.951</v>
       </c>
-      <c r="O6" s="22" t="n">
+      <c r="O6" s="23" t="n">
         <v>81</v>
       </c>
-      <c r="P6" s="22" t="n">
+      <c r="P6" s="23" t="n">
         <v>0.062</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="22" t="n">
+      <c r="R6" s="23" t="n">
         <v>0.007</v>
       </c>
-      <c r="S6" s="22" t="n">
+      <c r="S6" s="23" t="n">
         <v>0.206</v>
       </c>
-      <c r="T6" s="22" t="n">
+      <c r="T6" s="23" t="n">
         <v>94</v>
       </c>
-      <c r="U6" s="22" t="n">
+      <c r="U6" s="23" t="n">
         <v>1.276</v>
       </c>
-      <c r="V6" s="21" t="s">
+      <c r="V6" s="22" t="s">
         <v>20</v>
       </c>
       <c r="W6" s="1"/>
@@ -3192,20 +3214,20 @@
       <c r="I7" s="8" t="n">
         <v>0.725</v>
       </c>
-      <c r="J7" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="18" t="n">
+      <c r="J7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="19" t="n">
         <v>0.352</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="20" t="s">
         <v>20</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="21"/>
+      <c r="Q7" s="22"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -3238,16 +3260,16 @@
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24" t="s">
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="21"/>
+      <c r="Q8" s="22"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -3280,16 +3302,16 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19" t="s">
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="20" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="21"/>
+      <c r="Q9" s="22"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -3322,16 +3344,16 @@
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24" t="s">
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25" t="s">
         <v>40</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="21"/>
+      <c r="Q10" s="22"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -3364,16 +3386,16 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="19" t="s">
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="21"/>
+      <c r="Q11" s="22"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>

</xml_diff>

<commit_message>
adding ants and fsl
</commit_message>
<xml_diff>
--- a/dave-simple2.xlsx
+++ b/dave-simple2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="59">
   <si>
     <t xml:space="preserve">Our Result</t>
   </si>
@@ -347,17 +347,56 @@
     <t xml:space="preserve">GANJ-5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">{'PIET-1': {'P&gt;|t|': ' 0.001', 't': '    3.442', 'rsquared_adj': '0.104', 'nobs': '461'}, 'MAC-1': {'P&gt;|t|': ' 0.001', 't': '    3.217', 'rsquared_adj': '0.0822', 'nobs': '428'}, 'MAC-2': {'P&gt;|t|': ' 0.001', 't': '    3.341', 'rsquared_adj': '0.0918', 'nobs': '336'}, 'MAC-3': {'P&gt;|t|': ' 0.218', 't': '    1.243', 'rsquared_adj': '0.08', 'nobs': ' 92'}, 'GANJ-1': {'P&gt;|t|': ' 0.257', 't': '   -1.134', 'rsquared_adj': '0.0918', 'nobs': '428'}, 'GANJ-2': {'P&gt;|t|': ' 0.156', 't': '   -1.425', 'rsquared_adj': '0.0854', 'nobs': '188'}, 'GANJ-3': {'P&gt;|t|': ' 0.972', 't': '   -0.035', 'rsquared_adj': '0.0883', 'nobs': '355'}, 'GANJ-4': {'P&gt;|t|': ' 0.467', 't': '   -0.730', 'rsquared_adj': '0.097', 'nobs': '145'}, 'GANJ-5': {'P&gt;|t|': ' 0.520', 't': '   -0.650', 'rsquared_adj': '-0.102', 'nobs': ' 43'}}
+    <t xml:space="preserve">{'PIET-1': {'P&gt;|t|': ' 0.001', 't': '    3.442', 'rsquared_adj': '0.104', 'nobs': '461'}, 'MAC-1': {'P&gt;|t|': ' 0.001', 't': '    3.217', 'rsquared_adj': '0.0822', 'nobs': '428'}, 'MAC-2': {'P&gt;|t|': ' 0.001', 't': '    3.341', 'rsquared_adj': '0.0918', 'nobs': '336'}, 'MAC-3': {'P&gt;|t|': ' 0.218', 't': '    1.243', 'rsquared_adj': '0.08', 'nobs': ' 92'}, 'GANJ-1': {'P&gt;|t|': ' 0.257', 't': '   -1.134', 'rsquared_adj': '0.0918', 'nobs': '428'}, 'GANJ-2': {'P&gt;|t|': ' 0.156', 't': '   -1.425', 'rsquared_adj': '0.0854', 'nobs': '188'}, 'GANJ-3': {'P&gt;|t|': ' 0.972', 't': '   -0.035', 'rsquared_adj': '0.0883', 'nobs': '355'}, 'GANJ-4': {'P&gt;|t|': ' 0.467', 't': '   -0.730', 'rsquared_adj': '0.097', 'nobs': '145'}, 'GANJ-5': {'P&gt;|t|': ' 0.520', 't': '   -0.650', 'rsquared_adj': '-0.102', 'nobs': ' 43'}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 </t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">resdic
+{'PIET-1': {'P&gt;|t|': ' 0.020',
+  't': '    2.334',
+  'rsquared_adj': '0.0764',
+  'nobs': '573',
+  'conditions': ['fiq&gt;0', 'normDev', 'fsl']},
+ 'MAC-1': {'P&gt;|t|': ' 0.000',
+  't': '    4.352',
+  'rsquared_adj': '0.115',
+  'nobs': '455',
+  'conditions': ['fiq&gt;0', 'normDev', 'fsl', 'left', 'age&lt;20']},
+ 'MAC-2': {'P&gt;|t|': ' 0.000',
+  't': '    4.258',
+  'rsquared_adj': '0.128',
+  'nobs': '364',
+  'conditions': ['fiq&gt;0', 'normDev', 'fsl', 'left', 'age&lt;20', 'male']},
+ 'MAC-3': {'P&gt;|t|': ' 0.201',
+  't': '    1.290',
+  'rsquared_adj': '0.0781',
+  'nobs': ' 91',
+  'conditions': ['fiq&gt;0', 'normDev', 'fsl', 'left', 'age&lt;20', 'female']}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'PIET-1': {'P&gt;|t|': ' 0.001',
+  't': '    3.442',
+  'rsquared_adj': '0.104',
+  'nobs': '461',
+  'conditions': ['bvol', 'fiq&gt;0', 'normDev', 'ants']},
+ 'MAC-1': {'P&gt;|t|': ' 0.001',
+  't': '    3.419',
+  'rsquared_adj': '0.116',
+  'nobs': '407',
+  'conditions': ['fiq&gt;0', 'normDev', 'ants', 'left', 'age&lt;20']},
+ 'MAC-2': {'P&gt;|t|': ' 0.000',
+  't': '    3.732',
+  'rsquared_adj': '0.139',
+  'nobs': '326',
+  'conditions': ['fiq&gt;0', 'normDev', 'ants', 'left', 'age&lt;20', 'male']},
+ 'MAC-3': {'P&gt;|t|': ' 0.545',
+  't': '    0.609',
+  'rsquared_adj': '0.0509',
+  'nobs': ' 81',
+  'conditions': ['fiq&gt;0', 'normDev', 'ants', 'left', 'age&lt;20', 'female']}}</t>
   </si>
   <si>
     <t xml:space="preserve">Our Result (FS )</t>
@@ -544,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -613,7 +652,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -726,10 +773,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1791,14 +1838,25 @@
     </row>
     <row r="23" customFormat="false" ht="38.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C24" s="17" t="s">
+      <c r="A24" s="17" t="s">
         <v>48</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2821,21 +2879,21 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="M1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -2867,7 +2925,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
@@ -2878,11 +2936,11 @@
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>8</v>
@@ -2893,11 +2951,11 @@
       <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>8</v>
@@ -2942,30 +3000,30 @@
         <v>0.073</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="19" t="n">
+        <v>56</v>
+      </c>
+      <c r="J3" s="21" t="n">
         <v>515</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="K3" s="21" t="n">
         <v>3.674</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="21" t="n">
+      <c r="M3" s="23" t="n">
         <v>0.092</v>
       </c>
-      <c r="N3" s="21" t="n">
+      <c r="N3" s="23" t="n">
         <v>0.001</v>
       </c>
-      <c r="O3" s="21" t="n">
+      <c r="O3" s="23" t="n">
         <v>458</v>
       </c>
-      <c r="P3" s="21" t="n">
+      <c r="P3" s="23" t="n">
         <v>3.478</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="24" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="10"/>
@@ -3007,40 +3065,40 @@
       <c r="J4" s="12" t="n">
         <v>409</v>
       </c>
-      <c r="K4" s="19" t="n">
+      <c r="K4" s="21" t="n">
         <v>2.913</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="23" t="n">
+      <c r="M4" s="25" t="n">
         <v>0.095</v>
       </c>
-      <c r="N4" s="23" t="n">
+      <c r="N4" s="25" t="n">
         <v>0.003</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="25" t="n">
         <v>407</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="25" t="n">
         <v>3.019</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="R4" s="25" t="n">
         <v>0.106</v>
       </c>
-      <c r="S4" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" s="23" t="n">
+      <c r="S4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="25" t="n">
         <v>457</v>
       </c>
-      <c r="U4" s="23" t="n">
+      <c r="U4" s="25" t="n">
         <v>4.246</v>
       </c>
-      <c r="V4" s="22" t="s">
+      <c r="V4" s="24" t="s">
         <v>20</v>
       </c>
       <c r="W4" s="1"/>
@@ -3074,43 +3132,43 @@
       <c r="I5" s="8" t="n">
         <v>0.002</v>
       </c>
-      <c r="J5" s="19" t="n">
+      <c r="J5" s="21" t="n">
         <v>321</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="K5" s="21" t="n">
         <v>3.152</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="23" t="n">
+      <c r="M5" s="25" t="n">
         <v>0.121</v>
       </c>
-      <c r="N5" s="23" t="n">
+      <c r="N5" s="25" t="n">
         <v>0.001</v>
       </c>
-      <c r="O5" s="23" t="n">
+      <c r="O5" s="25" t="n">
         <v>326</v>
       </c>
-      <c r="P5" s="23" t="n">
+      <c r="P5" s="25" t="n">
         <v>3.44</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="23" t="n">
+      <c r="R5" s="25" t="n">
         <v>0.124</v>
       </c>
-      <c r="S5" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5" s="23" t="n">
+      <c r="S5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="25" t="n">
         <v>363</v>
       </c>
-      <c r="U5" s="23" t="n">
+      <c r="U5" s="25" t="n">
         <v>4.217</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" s="24" t="s">
         <v>20</v>
       </c>
       <c r="W5" s="1"/>
@@ -3144,43 +3202,43 @@
       <c r="I6" s="8" t="n">
         <v>0.608</v>
       </c>
-      <c r="J6" s="19" t="n">
+      <c r="J6" s="21" t="n">
         <v>88</v>
       </c>
-      <c r="K6" s="19" t="n">
+      <c r="K6" s="21" t="n">
         <v>0.516</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="23" t="n">
+      <c r="M6" s="25" t="n">
         <v>-0.023</v>
       </c>
-      <c r="N6" s="23" t="n">
+      <c r="N6" s="25" t="n">
         <v>0.951</v>
       </c>
-      <c r="O6" s="23" t="n">
+      <c r="O6" s="25" t="n">
         <v>81</v>
       </c>
-      <c r="P6" s="23" t="n">
+      <c r="P6" s="25" t="n">
         <v>0.062</v>
       </c>
-      <c r="Q6" s="22" t="s">
+      <c r="Q6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="23" t="n">
+      <c r="R6" s="25" t="n">
         <v>0.007</v>
       </c>
-      <c r="S6" s="23" t="n">
+      <c r="S6" s="25" t="n">
         <v>0.206</v>
       </c>
-      <c r="T6" s="23" t="n">
+      <c r="T6" s="25" t="n">
         <v>94</v>
       </c>
-      <c r="U6" s="23" t="n">
+      <c r="U6" s="25" t="n">
         <v>1.276</v>
       </c>
-      <c r="V6" s="22" t="s">
+      <c r="V6" s="24" t="s">
         <v>20</v>
       </c>
       <c r="W6" s="1"/>
@@ -3214,20 +3272,20 @@
       <c r="I7" s="8" t="n">
         <v>0.725</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="19" t="n">
+      <c r="J7" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="21" t="n">
         <v>0.352</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="22" t="s">
         <v>20</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="22"/>
+      <c r="Q7" s="24"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -3260,16 +3318,16 @@
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25" t="s">
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="22"/>
+      <c r="Q8" s="24"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -3302,16 +3360,16 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20" t="s">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="22" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="22"/>
+      <c r="Q9" s="24"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -3344,16 +3402,16 @@
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25" t="s">
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27" t="s">
         <v>40</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="22"/>
+      <c r="Q10" s="24"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -3386,16 +3444,16 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="20" t="s">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="22" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="22"/>
+      <c r="Q11" s="24"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>

</xml_diff>